<commit_message>
separate ontologies related to project and remove nan values.
</commit_message>
<xml_diff>
--- a/MSE_ontologies.xlsx
+++ b/MSE_ontologies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="201">
   <si>
     <t>Materials Science and Engineering Ontology</t>
   </si>
@@ -546,6 +546,87 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.sciencedirect.com/topics/computer-science/data-ontology </t>
+  </si>
+  <si>
+    <t>Ontology file</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/materialdigital/core-ontology/main/pmdco_core.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/domain-mechanical-testing/master/emmo-mechanical-testing.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/jesper-friis/emmo-microstructure/master/emmo-microstructure.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/EMMO/master/emmo.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/BFO-ontology/BFO-2020/master/21838-2/owl/bfo-2020.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/oeg-upm/SMART-Protocols/master/wfProtocolV2.0.owl</t>
+  </si>
+  <si>
+    <t>https://gitlab.cc-asp.fraunhofer.de/EMI_datamanagement/bwmd_ontology/-/raw/master/BWMD_domain.owl</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/prov-o.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/General-Process-Ontology/ontology/master/GPO_inferred.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Battery-Value-Chain-Ontology/ontology/master/BVCO.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/domain-crystallography/master/crystallography.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/datamodel-ontology/master/datamodel.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/domain-mappings/master/mappings.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/inovexcorp/MatOnto-Ontologies/master/matonto.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/domain-atomistic/master/atomistic.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/sobolevnrm/npo/master/npo-inferred.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/enanomapper/ontologies/master/enanomapper.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/daimoners/MAMBO/master/mambo.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/cpauloh/semmd/master/skos/mmd_skos_vocab.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/BIG-MAP/BattINFO/master/battinfo.ttl</t>
+  </si>
+  <si>
+    <t>http://www.daml.org/2003/01/periodictable/PeriodicTable.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ProjectDebbie/Ontology_DEB/master/DEB_ont.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/tetherless-world/nanomine-ontology/master/nanomine.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Materials-Data-Science-and-Informatics/dislocation-ontology/master/dislocation-ontology.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/LiUSemWeb/Materials-Design-Ontology/master/mdo-full.owl</t>
+  </si>
+  <si>
+    <t>http://home.agh.edu.pl/~pmaciol/wordpress/wp-content/uploads/metal-alloy.zip</t>
   </si>
 </sst>
 </file>
@@ -663,7 +744,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -716,6 +797,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -723,7 +808,10 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -783,16 +871,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H41" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H41"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Materials Science and Engineering Ontology" dataDxfId="7"/>
-    <tableColumn id="8" name="Short Name" dataDxfId="6"/>
-    <tableColumn id="2" name="Domain" dataDxfId="5"/>
-    <tableColumn id="3" name="Last update" dataDxfId="4"/>
-    <tableColumn id="4" name="Number of classes" dataDxfId="3"/>
-    <tableColumn id="5" name="Number of properties" dataDxfId="2"/>
-    <tableColumn id="6" name="Reference (Ontology)" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:I41" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I41"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Materials Science and Engineering Ontology" dataDxfId="8"/>
+    <tableColumn id="8" name="Short Name" dataDxfId="7"/>
+    <tableColumn id="2" name="Domain" dataDxfId="6"/>
+    <tableColumn id="3" name="Last update" dataDxfId="5"/>
+    <tableColumn id="4" name="Number of classes" dataDxfId="4"/>
+    <tableColumn id="5" name="Number of properties" dataDxfId="3"/>
+    <tableColumn id="6" name="Reference (Ontology)" dataDxfId="2"/>
+    <tableColumn id="9" name="Ontology file" dataDxfId="1" dataCellStyle="Link"/>
     <tableColumn id="7" name="Reference (Paper)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1062,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,11 +1166,12 @@
     <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="55.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.5703125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="3"/>
+    <col min="8" max="8" width="55.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="49.5703125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1104,10 +1194,13 @@
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>124</v>
       </c>
@@ -1131,10 +1224,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
@@ -1157,8 +1253,11 @@
       <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1181,8 +1280,11 @@
       <c r="G4" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1204,8 +1306,11 @@
       <c r="G5" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>130</v>
       </c>
@@ -1228,10 +1333,13 @@
         <v>56</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>135</v>
       </c>
@@ -1253,8 +1361,9 @@
       <c r="G7" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>82</v>
       </c>
@@ -1277,8 +1386,11 @@
       <c r="G8" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>127</v>
       </c>
@@ -1300,8 +1412,11 @@
       <c r="G9" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>144</v>
       </c>
@@ -1324,8 +1439,11 @@
       <c r="G10" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>145</v>
       </c>
@@ -1348,8 +1466,11 @@
       <c r="G11" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -1370,8 +1491,9 @@
         <v>317</v>
       </c>
       <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>146</v>
       </c>
@@ -1387,11 +1509,12 @@
       <c r="G13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>148</v>
       </c>
@@ -1414,8 +1537,11 @@
       <c r="G14" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H14" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
@@ -1438,8 +1564,11 @@
       <c r="G15" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>150</v>
       </c>
@@ -1461,8 +1590,11 @@
       <c r="G16" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1484,8 +1616,11 @@
       <c r="G17" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1508,8 +1643,11 @@
       <c r="G18" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1533,10 +1671,13 @@
         <v>46</v>
       </c>
       <c r="H19" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1559,8 +1700,11 @@
       <c r="G20" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1583,8 +1727,11 @@
       <c r="G21" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
@@ -1607,10 +1754,13 @@
         <v>60</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -1621,11 +1771,11 @@
         <v>62</v>
       </c>
       <c r="D23" s="15"/>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
@@ -1642,18 +1792,18 @@
       <c r="F24" s="6">
         <v>31</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="18" t="s">
         <v>172</v>
       </c>
       <c r="D25" s="15"/>
@@ -1663,11 +1813,11 @@
       <c r="F25" s="6">
         <v>37</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
@@ -1690,10 +1840,13 @@
         <v>53</v>
       </c>
       <c r="H26" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -1717,10 +1870,13 @@
         <v>66</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
@@ -1737,11 +1893,11 @@
       <c r="F28" s="3">
         <v>9</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>156</v>
       </c>
@@ -1765,10 +1921,13 @@
         <v>75</v>
       </c>
       <c r="H29" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I29" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>20</v>
       </c>
@@ -1792,10 +1951,13 @@
         <v>72</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -1818,10 +1980,13 @@
         <v>19</v>
       </c>
       <c r="H31" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I31" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
@@ -1842,10 +2007,13 @@
         <v>119</v>
       </c>
       <c r="H32" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>158</v>
       </c>
@@ -1868,10 +2036,13 @@
         <v>114</v>
       </c>
       <c r="H33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>110</v>
       </c>
@@ -1888,10 +2059,13 @@
         <v>113</v>
       </c>
       <c r="H34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
@@ -1912,8 +2086,9 @@
       <c r="G35" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>109</v>
       </c>
@@ -1927,11 +2102,12 @@
       <c r="G36" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H36" s="5"/>
+      <c r="I36" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>16</v>
       </c>
@@ -1954,8 +2130,11 @@
       <c r="G37" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
@@ -1975,8 +2154,11 @@
       <c r="G38" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>165</v>
       </c>
@@ -2000,10 +2182,13 @@
         <v>22</v>
       </c>
       <c r="H39" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>120</v>
       </c>
@@ -2019,8 +2204,11 @@
       <c r="G40" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2103,78 +2291,90 @@
       <c r="C63" s="9"/>
       <c r="D63" s="17"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
       <c r="C65" s="9"/>
       <c r="D65" s="12"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
       <c r="C67" s="9"/>
       <c r="D67" s="12"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
       <c r="C68" s="9"/>
       <c r="D68" s="12"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G69" s="13"/>
-      <c r="H69" s="14"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H22" r:id="rId1"/>
-    <hyperlink ref="H31" r:id="rId2"/>
+    <hyperlink ref="I22" r:id="rId1"/>
+    <hyperlink ref="I31" r:id="rId2"/>
     <hyperlink ref="G31" r:id="rId3"/>
     <hyperlink ref="G39" r:id="rId4"/>
-    <hyperlink ref="H39" r:id="rId5"/>
+    <hyperlink ref="I39" r:id="rId5"/>
     <hyperlink ref="G17" r:id="rId6"/>
     <hyperlink ref="G16" r:id="rId7"/>
     <hyperlink ref="G18" r:id="rId8"/>
-    <hyperlink ref="H19" r:id="rId9"/>
+    <hyperlink ref="I19" r:id="rId9"/>
     <hyperlink ref="G19" r:id="rId10"/>
     <hyperlink ref="G20" r:id="rId11"/>
     <hyperlink ref="G21" r:id="rId12"/>
-    <hyperlink ref="H26" r:id="rId13"/>
+    <hyperlink ref="I26" r:id="rId13"/>
     <hyperlink ref="G26" r:id="rId14"/>
     <hyperlink ref="G22" r:id="rId15"/>
-    <hyperlink ref="H23" r:id="rId16"/>
-    <hyperlink ref="H27" r:id="rId17"/>
+    <hyperlink ref="I23" r:id="rId16"/>
+    <hyperlink ref="I27" r:id="rId17"/>
     <hyperlink ref="G27" r:id="rId18"/>
-    <hyperlink ref="H28" r:id="rId19"/>
-    <hyperlink ref="H30" r:id="rId20"/>
+    <hyperlink ref="I28" r:id="rId19"/>
+    <hyperlink ref="I30" r:id="rId20"/>
     <hyperlink ref="G30" r:id="rId21"/>
-    <hyperlink ref="H29" r:id="rId22"/>
+    <hyperlink ref="I29" r:id="rId22"/>
     <hyperlink ref="G29" r:id="rId23"/>
-    <hyperlink ref="H24" r:id="rId24"/>
+    <hyperlink ref="I24" r:id="rId24"/>
     <hyperlink ref="G37" r:id="rId25"/>
     <hyperlink ref="G13" r:id="rId26"/>
-    <hyperlink ref="H13" r:id="rId27"/>
+    <hyperlink ref="I13" r:id="rId27"/>
     <hyperlink ref="G14" r:id="rId28"/>
     <hyperlink ref="G15" r:id="rId29"/>
     <hyperlink ref="G35" r:id="rId30" location="OntologyDescription "/>
     <hyperlink ref="G38" r:id="rId31"/>
     <hyperlink ref="G36" r:id="rId32"/>
-    <hyperlink ref="H36" r:id="rId33"/>
-    <hyperlink ref="H34" r:id="rId34"/>
+    <hyperlink ref="I36" r:id="rId33"/>
+    <hyperlink ref="I34" r:id="rId34"/>
     <hyperlink ref="G34" r:id="rId35"/>
     <hyperlink ref="G33" r:id="rId36"/>
-    <hyperlink ref="H33" r:id="rId37"/>
-    <hyperlink ref="H32" r:id="rId38"/>
+    <hyperlink ref="I33" r:id="rId37"/>
+    <hyperlink ref="I32" r:id="rId38"/>
     <hyperlink ref="G32" r:id="rId39"/>
     <hyperlink ref="G40" r:id="rId40"/>
     <hyperlink ref="G4" r:id="rId41"/>
     <hyperlink ref="G5" r:id="rId42"/>
-    <hyperlink ref="H25" r:id="rId43"/>
+    <hyperlink ref="I25" r:id="rId43"/>
+    <hyperlink ref="G2" r:id="rId44"/>
+    <hyperlink ref="G3" r:id="rId45"/>
+    <hyperlink ref="G6" r:id="rId46"/>
+    <hyperlink ref="G7" r:id="rId47"/>
+    <hyperlink ref="G8" r:id="rId48"/>
+    <hyperlink ref="G9" r:id="rId49"/>
+    <hyperlink ref="G10" r:id="rId50"/>
+    <hyperlink ref="G11" r:id="rId51"/>
+    <hyperlink ref="H15" r:id="rId52"/>
+    <hyperlink ref="H34" r:id="rId53"/>
+    <hyperlink ref="H38" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
   <tableParts count="1">
-    <tablePart r:id="rId45"/>
+    <tablePart r:id="rId56"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update a namespace issue from rdflib
</commit_message>
<xml_diff>
--- a/MSE_ontologies.xlsx
+++ b/MSE_ontologies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="204">
   <si>
     <t>Materials Science and Engineering Ontology</t>
   </si>
@@ -263,9 +263,6 @@
     <t xml:space="preserve">Specification of all metadata terms </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dublincore.org/specifications/dublin-core/dcmi-terms/ </t>
-  </si>
-  <si>
     <t>Describe people and social relationship on the Web</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>Representation of the Periodic Table of the Elements</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/CommonCoreOntology/CommonCoreOntologies </t>
-  </si>
-  <si>
     <t>Comprise twelve ontologies that contain classes and relations that are used in many domains of interest.</t>
   </si>
   <si>
@@ -467,9 +461,6 @@
     <t>Common Core Ontology</t>
   </si>
   <si>
-    <t>BWM</t>
-  </si>
-  <si>
     <t>Baden Württemberg Material Digital Ontology</t>
   </si>
   <si>
@@ -584,21 +575,12 @@
     <t>https://raw.githubusercontent.com/emmo-repo/domain-crystallography/master/crystallography.ttl</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/emmo-repo/datamodel-ontology/master/datamodel.ttl</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/emmo-repo/domain-mappings/master/mappings.ttl</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/inovexcorp/MatOnto-Ontologies/master/matonto.ttl</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/emmo-repo/domain-atomistic/master/atomistic.ttl</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/sobolevnrm/npo/master/npo-inferred.owl</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/enanomapper/ontologies/master/enanomapper.owl</t>
   </si>
   <si>
@@ -627,6 +609,33 @@
   </si>
   <si>
     <t>http://home.agh.edu.pl/~pmaciol/wordpress/wp-content/uploads/metal-alloy.zip</t>
+  </si>
+  <si>
+    <t>http://rest.matportal.org/ontologies/CCO/submissions/2/download?apikey=66c82e77-ce0d-4385-8056-a95898e47ebb</t>
+  </si>
+  <si>
+    <t>https://www.dublincore.org/specifications/dublin-core/dcmi-terms/dublin_core_terms.ttl</t>
+  </si>
+  <si>
+    <t>https://github.com/Mat-O-Lab/MSEO</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Mat-O-Lab/MSEO/main/MSEO_mid.ttl</t>
+  </si>
+  <si>
+    <t>https://www.dublincore.org/specifications/dublin-core/dcmi-terms/</t>
+  </si>
+  <si>
+    <t>BWMD</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/datamodel-ontology/master/metamodel.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/inovexcorp/MatOnto-Ontologies/master/matonto-release.ttl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/sobolevnrm/npo/master/npo-asserted.owl</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1194,7 +1203,7 @@
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>27</v>
@@ -1202,7 +1211,7 @@
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -1224,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>25</v>
@@ -1232,10 +1241,10 @@
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>59</v>
@@ -1254,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1262,7 +1271,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
@@ -1281,7 +1290,7 @@
         <v>29</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1289,7 +1298,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>58</v>
@@ -1307,15 +1316,15 @@
         <v>57</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>55</v>
@@ -1333,7 +1342,7 @@
         <v>56</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>54</v>
@@ -1341,10 +1350,10 @@
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -1358,20 +1367,22 @@
       <c r="F7" s="6">
         <v>55</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" s="5"/>
+      <c r="G7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="D8" s="7">
         <v>44687</v>
@@ -1384,21 +1395,21 @@
         <v>23</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="7">
         <v>41976</v>
@@ -1410,21 +1421,21 @@
         <v>8</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="7">
         <v>41602</v>
@@ -1437,21 +1448,21 @@
         <v>8</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="7">
         <v>42974</v>
@@ -1464,21 +1475,21 @@
         <v>71</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="7">
         <v>44631</v>
@@ -1490,42 +1501,45 @@
         <f>287+30</f>
         <v>317</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="7">
         <v>44635</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>147</v>
+        <v>200</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E14" s="6">
         <v>787</v>
@@ -1535,21 +1549,21 @@
         <v>39</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="7">
         <v>41394</v>
@@ -1562,18 +1576,18 @@
         <v>50</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -1591,7 +1605,7 @@
         <v>41</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1599,7 +1613,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>39</v>
@@ -1617,7 +1631,7 @@
         <v>40</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1625,7 +1639,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>31</v>
@@ -1644,7 +1658,7 @@
         <v>43</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1652,7 +1666,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>45</v>
@@ -1671,7 +1685,7 @@
         <v>46</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>44</v>
@@ -1682,7 +1696,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>48</v>
@@ -1701,7 +1715,7 @@
         <v>47</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1709,7 +1723,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>50</v>
@@ -1728,7 +1742,7 @@
         <v>49</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1754,7 +1768,7 @@
         <v>60</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>15</v>
@@ -1780,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>77</v>
@@ -1801,10 +1815,10 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="6">
@@ -1814,7 +1828,7 @@
         <v>37</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1822,7 +1836,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>52</v>
@@ -1840,7 +1854,7 @@
         <v>53</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>51</v>
@@ -1851,7 +1865,7 @@
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>65</v>
@@ -1870,7 +1884,7 @@
         <v>66</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>64</v>
@@ -1899,10 +1913,10 @@
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>74</v>
@@ -1921,7 +1935,7 @@
         <v>75</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>73</v>
@@ -1932,7 +1946,7 @@
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>70</v>
@@ -1951,7 +1965,7 @@
         <v>72</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>71</v>
@@ -1962,7 +1976,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>69</v>
@@ -1980,7 +1994,7 @@
         <v>19</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>17</v>
@@ -1994,7 +2008,7 @@
         <v>42</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3">
         <v>1730</v>
@@ -2004,24 +2018,24 @@
         <v>215</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D33" s="8">
         <v>44349</v>
@@ -2033,47 +2047,47 @@
         <v>121</v>
       </c>
       <c r="G33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" s="8">
         <v>43040</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="3">
@@ -2084,27 +2098,27 @@
         <v>174</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D36" s="16"/>
       <c r="G36" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2112,10 +2126,10 @@
         <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="8">
         <v>38022</v>
@@ -2128,21 +2142,21 @@
         <v>13</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E38" s="3">
         <v>16</v>
@@ -2152,18 +2166,18 @@
         <v>30</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>23</v>
@@ -2182,7 +2196,7 @@
         <v>22</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>24</v>
@@ -2190,22 +2204,22 @@
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D40" s="8">
         <v>43054</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2341,7 +2355,7 @@
     <hyperlink ref="G29" r:id="rId23"/>
     <hyperlink ref="I24" r:id="rId24"/>
     <hyperlink ref="G37" r:id="rId25"/>
-    <hyperlink ref="G13" r:id="rId26"/>
+    <hyperlink ref="H13" r:id="rId26"/>
     <hyperlink ref="I13" r:id="rId27"/>
     <hyperlink ref="G14" r:id="rId28"/>
     <hyperlink ref="G15" r:id="rId29"/>
@@ -2362,7 +2376,7 @@
     <hyperlink ref="G2" r:id="rId44"/>
     <hyperlink ref="G3" r:id="rId45"/>
     <hyperlink ref="G6" r:id="rId46"/>
-    <hyperlink ref="G7" r:id="rId47"/>
+    <hyperlink ref="H7" r:id="rId47"/>
     <hyperlink ref="G8" r:id="rId48"/>
     <hyperlink ref="G9" r:id="rId49"/>
     <hyperlink ref="G10" r:id="rId50"/>
@@ -2370,11 +2384,14 @@
     <hyperlink ref="H15" r:id="rId52"/>
     <hyperlink ref="H34" r:id="rId53"/>
     <hyperlink ref="H38" r:id="rId54"/>
+    <hyperlink ref="H19" r:id="rId55"/>
+    <hyperlink ref="H22" r:id="rId56"/>
+    <hyperlink ref="H26" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
   <tableParts count="1">
-    <tablePart r:id="rId56"/>
+    <tablePart r:id="rId59"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>